<commit_message>
rename sheets in sql code gen
</commit_message>
<xml_diff>
--- a/AgileCodeGen/ExcelSqlCodeGen.xlsx
+++ b/AgileCodeGen/ExcelSqlCodeGen.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dm_78\Source\Repos\AgileCodeGeneration\AgileCodeGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8342491-E026-45FB-97D7-9B5A91550384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816209AA-B335-4855-8D08-552DB09F74D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{76008577-2001-4285-8564-779E7F50D205}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{76008577-2001-4285-8564-779E7F50D205}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables-Model" sheetId="1" r:id="rId1"/>
-    <sheet name="SQL-Code - Add new custom field" sheetId="2" r:id="rId2"/>
-    <sheet name="SQL-Code - Drop custom field" sheetId="3" r:id="rId3"/>
+    <sheet name="CodeGen-AddColumn" sheetId="2" r:id="rId2"/>
+    <sheet name="CodeGen-DeleteColumn" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -508,7 +508,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -746,7 +746,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>